<commit_message>
sửa chịn lại cột
</commit_message>
<xml_diff>
--- a/UnfilteredData/AppStoreReviews.xlsx
+++ b/UnfilteredData/AppStoreReviews.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ScanReview_Theards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ScanReview_Theards\UnfilteredData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C073CC-0B7A-4F66-97CD-FA8766E07C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36928AF-0D9D-4D2D-A7F6-8EDB8EC3C090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3968,7 +3968,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -4025,7 +4025,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4330,8 +4330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -4339,7 +4339,7 @@
     <col min="1" max="1" width="34.44140625" customWidth="1"/>
     <col min="2" max="2" width="29.109375" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="255.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16140,5 +16140,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>